<commit_message>
create sortsub program to separate
</commit_message>
<xml_diff>
--- a/data/總統-A05-4-候選人得票數一覽表-各投開票所(臺東縣).xlsx
+++ b/data/總統-A05-4-候選人得票數一覽表-各投開票所(臺東縣).xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dyu/Downloads/全國投開票所一覽表/總統副總統選舉/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dyu/PycharmProjects/TWelection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3DAB26-97A4-9F4E-BAF7-F0B804BB8EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2ED6E5-6E3A-D746-B561-C85DBDF9ACB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="臺東縣" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="650">
   <si>
     <t>第16任總統副總統選舉候選人在臺東縣各投開票所得票數一覽表</t>
   </si>
@@ -1997,18 +1996,6 @@
   </si>
   <si>
     <t>35.65</t>
-  </si>
-  <si>
-    <t>柯文哲</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>賴清德</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>侯友宜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2081,11 +2068,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2423,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q258"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41:Q43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="14"/>
@@ -2434,116 +2421,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" ht="15">
       <c r="A6" s="1" t="s">
@@ -4128,15 +4115,15 @@
       <c r="N41" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="O41" s="5">
+      <c r="O41" s="4">
         <f>D8/$G8</f>
         <v>0.26222222222222225</v>
       </c>
-      <c r="P41" s="5">
+      <c r="P41" s="4">
         <f t="shared" ref="P41:Q41" si="0">E8/$G8</f>
         <v>0.34222222222222221</v>
       </c>
-      <c r="Q41" s="5">
+      <c r="Q41" s="4">
         <f t="shared" si="0"/>
         <v>0.39555555555555555</v>
       </c>
@@ -4184,15 +4171,15 @@
       <c r="N42" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O42" s="5">
+      <c r="O42" s="4">
         <f t="shared" ref="O42:O45" si="1">D9/$G9</f>
         <v>0.2661290322580645</v>
       </c>
-      <c r="P42" s="5">
+      <c r="P42" s="4">
         <f t="shared" ref="P42:P45" si="2">E9/$G9</f>
         <v>0.30846774193548387</v>
       </c>
-      <c r="Q42" s="5">
+      <c r="Q42" s="4">
         <f t="shared" ref="Q42:Q45" si="3">F9/$G9</f>
         <v>0.42540322580645162</v>
       </c>
@@ -4240,15 +4227,15 @@
       <c r="N43" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="O43" s="5">
+      <c r="O43" s="4">
         <f t="shared" si="1"/>
         <v>0.24500665778961384</v>
       </c>
-      <c r="P43" s="5">
+      <c r="P43" s="4">
         <f t="shared" si="2"/>
         <v>0.33288948069241014</v>
       </c>
-      <c r="Q43" s="5">
+      <c r="Q43" s="4">
         <f t="shared" si="3"/>
         <v>0.42210386151797602</v>
       </c>
@@ -4296,15 +4283,15 @@
       <c r="N44" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="O44" s="5">
+      <c r="O44" s="4">
         <f t="shared" si="1"/>
         <v>0.22255639097744362</v>
       </c>
-      <c r="P44" s="5">
+      <c r="P44" s="4">
         <f t="shared" si="2"/>
         <v>0.34135338345864663</v>
       </c>
-      <c r="Q44" s="5">
+      <c r="Q44" s="4">
         <f t="shared" si="3"/>
         <v>0.43609022556390975</v>
       </c>
@@ -4352,15 +4339,15 @@
       <c r="N45" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="O45" s="5">
+      <c r="O45" s="4">
         <f t="shared" si="1"/>
         <v>0.17457627118644067</v>
       </c>
-      <c r="P45" s="5">
+      <c r="P45" s="4">
         <f t="shared" si="2"/>
         <v>0.44915254237288138</v>
       </c>
-      <c r="Q45" s="5">
+      <c r="Q45" s="4">
         <f t="shared" si="3"/>
         <v>0.37627118644067797</v>
       </c>
@@ -13759,115 +13746,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A535EE65-19F9-364E-9438-C9E6B0519806}">
-  <dimension ref="D10:R13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
-  <cols>
-    <col min="17" max="17" width="20.59765625" customWidth="1"/>
-    <col min="18" max="18" width="14.59765625" customWidth="1"/>
-    <col min="19" max="19" width="19.3984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="10" spans="4:18">
-      <c r="F10" t="s">
-        <v>650</v>
-      </c>
-      <c r="G10" t="s">
-        <v>651</v>
-      </c>
-      <c r="H10" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="11" spans="4:18" ht="15">
-      <c r="D11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.26222222222222225</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.34222222222222221</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0.39555555555555555</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="4:18" ht="15">
-      <c r="D12" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.2661290322580645</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0.30846774193548387</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0.42540322580645162</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="4:18" ht="15">
-      <c r="D13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.24500665778961384</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.33288948069241014</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.42210386151797602</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="2"/>
-      <c r="R13" t="e">
-        <f t="shared" ref="R13" si="0">#REF!/#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>